<commit_message>
commiting hide row and dates
</commit_message>
<xml_diff>
--- a/Project_1.xlsx
+++ b/Project_1.xlsx
@@ -495,7 +495,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U51"/>
+  <dimension ref="A1:V51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -609,6 +609,11 @@
           <t>Interns</t>
         </is>
       </c>
+      <c r="V1" s="12" t="inlineStr">
+        <is>
+          <t>originalIndex</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -698,6 +703,9 @@
       <c r="U2" t="n">
         <v>0</v>
       </c>
+      <c r="V2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -787,6 +795,9 @@
       <c r="U3" t="n">
         <v>0</v>
       </c>
+      <c r="V3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -876,6 +887,9 @@
       <c r="U4" t="n">
         <v>0</v>
       </c>
+      <c r="V4" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -965,6 +979,9 @@
       <c r="U5" t="n">
         <v>0</v>
       </c>
+      <c r="V5" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -1054,6 +1071,9 @@
       <c r="U6" t="n">
         <v>0</v>
       </c>
+      <c r="V6" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -1143,6 +1163,9 @@
       <c r="U7" t="n">
         <v>0</v>
       </c>
+      <c r="V7" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1232,6 +1255,9 @@
       <c r="U8" t="n">
         <v>0</v>
       </c>
+      <c r="V8" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1321,6 +1347,9 @@
       <c r="U9" t="n">
         <v>0</v>
       </c>
+      <c r="V9" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1410,6 +1439,9 @@
       <c r="U10" t="n">
         <v>0</v>
       </c>
+      <c r="V10" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1499,6 +1531,9 @@
       <c r="U11" t="n">
         <v>0</v>
       </c>
+      <c r="V11" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1588,6 +1623,9 @@
       <c r="U12" t="n">
         <v>0</v>
       </c>
+      <c r="V12" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1677,6 +1715,9 @@
       <c r="U13" t="n">
         <v>0</v>
       </c>
+      <c r="V13" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1766,6 +1807,9 @@
       <c r="U14" t="n">
         <v>0</v>
       </c>
+      <c r="V14" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1855,6 +1899,9 @@
       <c r="U15" t="n">
         <v>0</v>
       </c>
+      <c r="V15" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1944,6 +1991,9 @@
       <c r="U16" t="n">
         <v>0</v>
       </c>
+      <c r="V16" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -2033,6 +2083,9 @@
       <c r="U17" t="n">
         <v>0</v>
       </c>
+      <c r="V17" t="n">
+        <v>15</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -2122,6 +2175,9 @@
       <c r="U18" t="n">
         <v>0</v>
       </c>
+      <c r="V18" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -2211,6 +2267,9 @@
       <c r="U19" t="n">
         <v>0</v>
       </c>
+      <c r="V19" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -2300,6 +2359,9 @@
       <c r="U20" t="n">
         <v>0</v>
       </c>
+      <c r="V20" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -2389,6 +2451,9 @@
       <c r="U21" t="n">
         <v>0</v>
       </c>
+      <c r="V21" t="n">
+        <v>19</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -2478,6 +2543,9 @@
       <c r="U22" t="n">
         <v>0</v>
       </c>
+      <c r="V22" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -2567,6 +2635,9 @@
       <c r="U23" t="n">
         <v>0</v>
       </c>
+      <c r="V23" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -2656,6 +2727,9 @@
       <c r="U24" t="n">
         <v>0</v>
       </c>
+      <c r="V24" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -2745,6 +2819,9 @@
       <c r="U25" t="n">
         <v>0</v>
       </c>
+      <c r="V25" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -2834,6 +2911,9 @@
       <c r="U26" t="n">
         <v>0</v>
       </c>
+      <c r="V26" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -2923,6 +3003,9 @@
       <c r="U27" t="n">
         <v>0</v>
       </c>
+      <c r="V27" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -3012,6 +3095,9 @@
       <c r="U28" t="n">
         <v>0</v>
       </c>
+      <c r="V28" t="n">
+        <v>26</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -3101,6 +3187,9 @@
       <c r="U29" t="n">
         <v>0</v>
       </c>
+      <c r="V29" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -3190,6 +3279,9 @@
       <c r="U30" t="n">
         <v>0</v>
       </c>
+      <c r="V30" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -3279,6 +3371,9 @@
       <c r="U31" t="n">
         <v>0</v>
       </c>
+      <c r="V31" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -3368,6 +3463,9 @@
       <c r="U32" t="n">
         <v>0</v>
       </c>
+      <c r="V32" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -3457,6 +3555,9 @@
       <c r="U33" t="n">
         <v>0</v>
       </c>
+      <c r="V33" t="n">
+        <v>31</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -3546,6 +3647,9 @@
       <c r="U34" t="n">
         <v>0</v>
       </c>
+      <c r="V34" t="n">
+        <v>32</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -3635,6 +3739,9 @@
       <c r="U35" t="n">
         <v>0</v>
       </c>
+      <c r="V35" t="n">
+        <v>33</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -3724,6 +3831,9 @@
       <c r="U36" t="n">
         <v>0</v>
       </c>
+      <c r="V36" t="n">
+        <v>34</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -3813,6 +3923,9 @@
       <c r="U37" t="n">
         <v>0</v>
       </c>
+      <c r="V37" t="n">
+        <v>35</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -3902,6 +4015,9 @@
       <c r="U38" t="n">
         <v>0</v>
       </c>
+      <c r="V38" t="n">
+        <v>36</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -3991,6 +4107,9 @@
       <c r="U39" t="n">
         <v>0</v>
       </c>
+      <c r="V39" t="n">
+        <v>37</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -4080,6 +4199,9 @@
       <c r="U40" t="n">
         <v>0</v>
       </c>
+      <c r="V40" t="n">
+        <v>38</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -4169,6 +4291,9 @@
       <c r="U41" t="n">
         <v>0</v>
       </c>
+      <c r="V41" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -4258,6 +4383,9 @@
       <c r="U42" t="n">
         <v>0</v>
       </c>
+      <c r="V42" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -4347,6 +4475,9 @@
       <c r="U43" t="n">
         <v>0</v>
       </c>
+      <c r="V43" t="n">
+        <v>41</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -4436,6 +4567,9 @@
       <c r="U44" t="n">
         <v>0</v>
       </c>
+      <c r="V44" t="n">
+        <v>42</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -4525,6 +4659,9 @@
       <c r="U45" t="n">
         <v>0</v>
       </c>
+      <c r="V45" t="n">
+        <v>43</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -4614,6 +4751,9 @@
       <c r="U46" t="n">
         <v>0</v>
       </c>
+      <c r="V46" t="n">
+        <v>44</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -4703,6 +4843,9 @@
       <c r="U47" t="n">
         <v>0</v>
       </c>
+      <c r="V47" t="n">
+        <v>45</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -4792,6 +4935,9 @@
       <c r="U48" t="n">
         <v>0</v>
       </c>
+      <c r="V48" t="n">
+        <v>46</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -4881,6 +5027,9 @@
       <c r="U49" t="n">
         <v>0</v>
       </c>
+      <c r="V49" t="n">
+        <v>47</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -4970,6 +5119,9 @@
       <c r="U50" t="n">
         <v>0</v>
       </c>
+      <c r="V50" t="n">
+        <v>48</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -5041,11 +5193,22 @@
           <t>2023-12-20 00:00:00</t>
         </is>
       </c>
-      <c r="R51" t="inlineStr"/>
+      <c r="R51" t="inlineStr">
+        <is>
+          <t>12/25/2023</t>
+        </is>
+      </c>
       <c r="S51" t="inlineStr"/>
-      <c r="T51" t="inlineStr"/>
+      <c r="T51" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="U51" t="n">
         <v>0</v>
+      </c>
+      <c r="V51" t="n">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>